<commit_message>
🎨 Remove empty space and add 0 values
</commit_message>
<xml_diff>
--- a/export/scostamento_risorse.xlsx
+++ b/export/scostamento_risorse.xlsx
@@ -547,10 +547,18 @@
       <c r="D4" t="n">
         <v>133.875</v>
       </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
+      <c r="E4" t="n">
+        <v>-133.875</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -566,8 +574,12 @@
           <t>RIS14</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>76.5</v>
+      </c>
       <c r="F5" t="n">
         <v>76.5</v>
       </c>
@@ -595,10 +607,18 @@
       <c r="D6" t="n">
         <v>127.5</v>
       </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
+      <c r="E6" t="n">
+        <v>-127.5</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -614,8 +634,12 @@
           <t>RIS2</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>21.25</v>
+      </c>
       <c r="F7" t="n">
         <v>21.25</v>
       </c>
@@ -643,10 +667,18 @@
       <c r="D8" t="n">
         <v>306</v>
       </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
+      <c r="E8" t="n">
+        <v>-306</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -695,10 +727,18 @@
       <c r="D10" t="n">
         <v>127.5</v>
       </c>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
+      <c r="E10" t="n">
+        <v>-127.5</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -714,8 +754,12 @@
           <t>RIS12</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>42.5</v>
+      </c>
       <c r="F11" t="n">
         <v>42.5</v>
       </c>
@@ -743,10 +787,18 @@
       <c r="D12" t="n">
         <v>807.5</v>
       </c>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
+      <c r="E12" t="n">
+        <v>-807.5</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -765,10 +817,18 @@
       <c r="D13" t="n">
         <v>21.25</v>
       </c>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
+      <c r="E13" t="n">
+        <v>-21.25</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -847,10 +907,18 @@
       <c r="D16" t="n">
         <v>127.5</v>
       </c>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
+      <c r="E16" t="n">
+        <v>-127.5</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -866,8 +934,12 @@
           <t>RIS10</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>2703</v>
+      </c>
       <c r="F17" t="n">
         <v>2703</v>
       </c>
@@ -892,8 +964,12 @@
           <t>RIS6</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.425</v>
+      </c>
       <c r="F18" t="n">
         <v>0.425</v>
       </c>
@@ -918,8 +994,12 @@
           <t>RIS5</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>37275.135</v>
+      </c>
       <c r="F19" t="n">
         <v>37275.135</v>
       </c>
@@ -944,8 +1024,12 @@
           <t>RIS3</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>47.3025</v>
+      </c>
       <c r="F20" t="n">
         <v>47.3025</v>
       </c>
@@ -970,8 +1054,12 @@
           <t>RIS14</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>4197.81</v>
+      </c>
       <c r="F21" t="n">
         <v>4197.81</v>
       </c>
@@ -1059,10 +1147,18 @@
       <c r="D24" t="n">
         <v>37972.56</v>
       </c>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
+      <c r="E24" t="n">
+        <v>-37972.56</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1228,8 +1324,12 @@
           <t>RIS6</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr"/>
-      <c r="E30" t="inlineStr"/>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" t="n">
+        <v>5265.75</v>
+      </c>
       <c r="F30" t="n">
         <v>5265.75</v>
       </c>
@@ -1254,8 +1354,12 @@
           <t>RIS5</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr"/>
-      <c r="E31" t="inlineStr"/>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" t="n">
+        <v>89.25</v>
+      </c>
       <c r="F31" t="n">
         <v>89.25</v>
       </c>
@@ -1373,10 +1477,18 @@
       <c r="D35" t="n">
         <v>272</v>
       </c>
-      <c r="E35" t="inlineStr"/>
-      <c r="F35" t="inlineStr"/>
-      <c r="G35" t="inlineStr"/>
-      <c r="H35" t="inlineStr"/>
+      <c r="E35" t="n">
+        <v>-272</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -1542,8 +1654,12 @@
           <t>RIS3</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr"/>
-      <c r="E41" t="inlineStr"/>
+      <c r="D41" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" t="n">
+        <v>2171.2825</v>
+      </c>
       <c r="F41" t="n">
         <v>2171.2825</v>
       </c>
@@ -1601,10 +1717,18 @@
       <c r="D43" t="n">
         <v>153</v>
       </c>
-      <c r="E43" t="inlineStr"/>
-      <c r="F43" t="inlineStr"/>
-      <c r="G43" t="inlineStr"/>
-      <c r="H43" t="inlineStr"/>
+      <c r="E43" t="n">
+        <v>-153</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -1620,8 +1744,12 @@
           <t>RIS3</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr"/>
-      <c r="E44" t="inlineStr"/>
+      <c r="D44" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" t="n">
+        <v>4094.365</v>
+      </c>
       <c r="F44" t="n">
         <v>4094.365</v>
       </c>
@@ -1646,8 +1774,12 @@
           <t>RIS9</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr"/>
-      <c r="E45" t="inlineStr"/>
+      <c r="D45" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" t="n">
+        <v>21.25</v>
+      </c>
       <c r="F45" t="n">
         <v>21.25</v>
       </c>
@@ -1672,8 +1804,12 @@
           <t>RIS4</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr"/>
-      <c r="E46" t="inlineStr"/>
+      <c r="D46" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" t="n">
+        <v>552.5</v>
+      </c>
       <c r="F46" t="n">
         <v>552.5</v>
       </c>
@@ -1698,8 +1834,12 @@
           <t>RIS3</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr"/>
-      <c r="E47" t="inlineStr"/>
+      <c r="D47" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" t="n">
+        <v>31.875</v>
+      </c>
       <c r="F47" t="n">
         <v>31.875</v>
       </c>
@@ -1724,8 +1864,12 @@
           <t>RIS14</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr"/>
-      <c r="E48" t="inlineStr"/>
+      <c r="D48" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" t="n">
+        <v>425</v>
+      </c>
       <c r="F48" t="n">
         <v>425</v>
       </c>
@@ -1753,10 +1897,18 @@
       <c r="D49" t="n">
         <v>21.25</v>
       </c>
-      <c r="E49" t="inlineStr"/>
-      <c r="F49" t="inlineStr"/>
-      <c r="G49" t="inlineStr"/>
-      <c r="H49" t="inlineStr"/>
+      <c r="E49" t="n">
+        <v>-21.25</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -1772,8 +1924,12 @@
           <t>RIS12</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr"/>
-      <c r="E50" t="inlineStr"/>
+      <c r="D50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" t="n">
+        <v>875.16</v>
+      </c>
       <c r="F50" t="n">
         <v>875.16</v>
       </c>
@@ -1801,10 +1957,18 @@
       <c r="D51" t="n">
         <v>675.75</v>
       </c>
-      <c r="E51" t="inlineStr"/>
-      <c r="F51" t="inlineStr"/>
-      <c r="G51" t="inlineStr"/>
-      <c r="H51" t="inlineStr"/>
+      <c r="E51" t="n">
+        <v>-675.75</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H51" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -1820,8 +1984,12 @@
           <t>RIS1</t>
         </is>
       </c>
-      <c r="D52" t="inlineStr"/>
-      <c r="E52" t="inlineStr"/>
+      <c r="D52" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" t="n">
+        <v>459</v>
+      </c>
       <c r="F52" t="n">
         <v>459</v>
       </c>

</xml_diff>